<commit_message>
Added International Brand Exclusion
</commit_message>
<xml_diff>
--- a/data/agility/hofor_agility.xlsx
+++ b/data/agility/hofor_agility.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Projects\Gijos\EB Scraping\Dashboard\data\agility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{173205D7-2FDF-4FC5-B013-5A6C7FB3D3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E80D1CE-6588-4F6C-AA82-8B21CBD21D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,7 +1348,7 @@
         <v>1634874</v>
       </c>
       <c r="K2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L2" t="s">
         <v>102</v>
@@ -1473,7 +1473,7 @@
         <v>1634874</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" t="s">
         <v>102</v>
@@ -1705,7 +1705,7 @@
         <v>303692</v>
       </c>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L5" t="s">
         <v>103</v>
@@ -1827,7 +1827,7 @@
         <v>935122</v>
       </c>
       <c r="K6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" t="s">
         <v>104</v>
@@ -2086,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" t="s">
         <v>102</v>
@@ -2208,7 +2208,7 @@
         <v>1173924</v>
       </c>
       <c r="K9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" t="s">
         <v>105</v>
@@ -2333,7 +2333,7 @@
         <v>1173924</v>
       </c>
       <c r="K10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" t="s">
         <v>105</v>
@@ -2458,7 +2458,7 @@
         <v>1173924</v>
       </c>
       <c r="K11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" t="s">
         <v>105</v>
@@ -2583,7 +2583,7 @@
         <v>1634874</v>
       </c>
       <c r="K12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" t="s">
         <v>102</v>
@@ -2705,7 +2705,7 @@
         <v>1173924</v>
       </c>
       <c r="K13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L13" t="s">
         <v>105</v>
@@ -2827,7 +2827,7 @@
         <v>935122</v>
       </c>
       <c r="K14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L14" t="s">
         <v>104</v>

</xml_diff>